<commit_message>
Updated to start to handle masters
</commit_message>
<xml_diff>
--- a/fg/external_files/the_masters_picks.xlsx
+++ b/fg/external_files/the_masters_picks.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alexevans/Desktop/Projects/fgolf/fg/external_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40FEFF88-07F1-D54B-8011-F07B0FF6C7A6}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13B94032-C2FE-2440-BE4B-42F9DA5A581D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8520" yWindow="960" windowWidth="20280" windowHeight="15920" xr2:uid="{45295F2B-EB9E-3348-9AE2-9104864DF200}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16420" xr2:uid="{45295F2B-EB9E-3348-9AE2-9104864DF200}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="50">
   <si>
     <t>A</t>
   </si>
@@ -45,12 +45,21 @@
     <t>D</t>
   </si>
   <si>
+    <t>Rory McIlroy</t>
+  </si>
+  <si>
+    <t>Ian Poulter</t>
+  </si>
+  <si>
     <t>John Griffin</t>
   </si>
   <si>
     <t>Tiger Woods</t>
   </si>
   <si>
+    <t>Eddie Pepperell</t>
+  </si>
+  <si>
     <t>Andy Davis</t>
   </si>
   <si>
@@ -96,7 +105,82 @@
     <t>PERSON</t>
   </si>
   <si>
+    <t>Rafael Cabrera Bello</t>
+  </si>
+  <si>
+    <t>Alexander Noren</t>
+  </si>
+  <si>
     <t>Dustin Johnson</t>
+  </si>
+  <si>
+    <t>Brooks Koepka</t>
+  </si>
+  <si>
+    <t>Rickie Fowler</t>
+  </si>
+  <si>
+    <t>Justin Rose</t>
+  </si>
+  <si>
+    <t>Xander Schauffele</t>
+  </si>
+  <si>
+    <t>Gary Woodland</t>
+  </si>
+  <si>
+    <t>Matthew Fitzpatrick</t>
+  </si>
+  <si>
+    <t>Kevin Kisner</t>
+  </si>
+  <si>
+    <t>Louis Oosthuizen</t>
+  </si>
+  <si>
+    <t>Brandt Snedeker</t>
+  </si>
+  <si>
+    <t>Patrick Cantlay</t>
+  </si>
+  <si>
+    <t>Kiradech Aphibarnrat</t>
+  </si>
+  <si>
+    <t>Cameron Smith</t>
+  </si>
+  <si>
+    <t>Shane Lowry</t>
+  </si>
+  <si>
+    <t>Corey Conners</t>
+  </si>
+  <si>
+    <t>Satoshi Kodaira</t>
+  </si>
+  <si>
+    <t>Lucas Bjerregaard</t>
+  </si>
+  <si>
+    <t>Justin Harding</t>
+  </si>
+  <si>
+    <t>Mike Weir</t>
+  </si>
+  <si>
+    <t>Adam Long</t>
+  </si>
+  <si>
+    <t>Vijay Singh</t>
+  </si>
+  <si>
+    <t>Devon Bling</t>
+  </si>
+  <si>
+    <t>Sandy Lyle</t>
+  </si>
+  <si>
+    <t>Li Haotong</t>
   </si>
 </sst>
 </file>
@@ -451,7 +535,7 @@
   <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -465,7 +549,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -482,92 +566,257 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>6</v>
+        <v>9</v>
+      </c>
+      <c r="B2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E2" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>7</v>
+        <v>10</v>
+      </c>
+      <c r="B3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D3" t="s">
+        <v>36</v>
+      </c>
+      <c r="E3" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>8</v>
+        <v>11</v>
+      </c>
+      <c r="B4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" t="s">
+        <v>38</v>
+      </c>
+      <c r="E4" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>9</v>
+        <v>12</v>
+      </c>
+      <c r="B5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" t="s">
+        <v>33</v>
+      </c>
+      <c r="D5" t="s">
+        <v>39</v>
+      </c>
+      <c r="E5" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>10</v>
+        <v>13</v>
+      </c>
+      <c r="B6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" t="s">
+        <v>30</v>
+      </c>
+      <c r="D6" t="s">
+        <v>49</v>
+      </c>
+      <c r="E6" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>11</v>
+        <v>14</v>
+      </c>
+      <c r="B7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" t="s">
+        <v>30</v>
+      </c>
+      <c r="D7" t="s">
+        <v>36</v>
+      </c>
+      <c r="E7" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>12</v>
+        <v>15</v>
+      </c>
+      <c r="B8" t="s">
+        <v>28</v>
+      </c>
+      <c r="C8" t="s">
+        <v>34</v>
+      </c>
+      <c r="D8" t="s">
+        <v>40</v>
+      </c>
+      <c r="E8" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>13</v>
+        <v>16</v>
+      </c>
+      <c r="B9" t="s">
+        <v>4</v>
+      </c>
+      <c r="C9" t="s">
+        <v>33</v>
+      </c>
+      <c r="D9" t="s">
+        <v>37</v>
+      </c>
+      <c r="E9" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="B10" t="s">
-        <v>21</v>
+        <v>26</v>
+      </c>
+      <c r="C10" t="s">
+        <v>35</v>
+      </c>
+      <c r="D10" t="s">
+        <v>38</v>
+      </c>
+      <c r="E10" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="B11" t="s">
-        <v>21</v>
+        <v>26</v>
+      </c>
+      <c r="C11" t="s">
+        <v>30</v>
+      </c>
+      <c r="D11" t="s">
+        <v>36</v>
+      </c>
+      <c r="E11" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B12" t="s">
-        <v>5</v>
+        <v>7</v>
+      </c>
+      <c r="C12" t="s">
+        <v>31</v>
+      </c>
+      <c r="D12" t="s">
+        <v>36</v>
+      </c>
+      <c r="E12" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>16</v>
+        <v>19</v>
+      </c>
+      <c r="B13" t="s">
+        <v>4</v>
+      </c>
+      <c r="C13" t="s">
+        <v>34</v>
+      </c>
+      <c r="D13" t="s">
+        <v>38</v>
+      </c>
+      <c r="E13" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>17</v>
+        <v>20</v>
+      </c>
+      <c r="B14" t="s">
+        <v>4</v>
+      </c>
+      <c r="C14" t="s">
+        <v>34</v>
+      </c>
+      <c r="D14" t="s">
+        <v>36</v>
+      </c>
+      <c r="E14" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="B15" t="s">
-        <v>5</v>
+        <v>7</v>
+      </c>
+      <c r="C15" t="s">
+        <v>30</v>
+      </c>
+      <c r="D15" t="s">
+        <v>8</v>
+      </c>
+      <c r="E15" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="B16" t="s">
-        <v>5</v>
+        <v>7</v>
+      </c>
+      <c r="C16" t="s">
+        <v>32</v>
+      </c>
+      <c r="D16" t="s">
+        <v>37</v>
+      </c>
+      <c r="E16" t="s">
+        <v>41</v>
       </c>
     </row>
   </sheetData>

</xml_diff>